<commit_message>
update tasks for 3 sem
</commit_message>
<xml_diff>
--- a/Tasks_3_sem/Tasks_3.xlsx
+++ b/Tasks_3_sem/Tasks_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Проги\Practice\Tasks_3_sem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA929E03-57CB-439C-906D-4A3EFCD0D7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5161C91A-E8E7-4D40-9E3A-48959C239D28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Начальное условие задачи</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Отредактированное условие</t>
   </si>
@@ -37,40 +34,323 @@
   </si>
   <si>
     <t>Теги</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Входные данные:                                                            Выходные данные: </t>
   </si>
   <si>
     <t>Дана строка вида (){}[]{}{})(){)))
 Необходимо проверить, что:
-1. Для каждой открывающей скобки есть соответственная закрывающая
+1. Для каждой открывающей скобки есть соответственная закрывающая;
 2. Не возникает ситуаций вида ( { ) } — скобки закрываются "не там".
-Если условия не выполнены, вывести, по какому индексу в строке произошла ошибка. Реализовать с помощью std::stack</t>
-  </si>
-  <si>
-    <t>Первая строка входного файла,задаваемого первым аргументом командой строки, содержит одно четное натуральное число N. Вторая строка входного файла содержит ровно N чисел - числа, написанные на игральных карточках. Все числа в строке разделяются одиночными пробелами. Игроки выбирают закрытые карточки, первый выбирает половину карточек, второй забирает оставшуюся половину. В файл, задаваемый вторым аргументом командной строки, записать максимальный выигрыш, который можно получить, т.е разница между суммами чисел на карточках. Примечание: sort()/partial_sort(), reverve(), accumulate(), std::greater</t>
-  </si>
-  <si>
-    <t>В единственной строке входного файла, задаваемого первым аргументом командной строки, находится последовательность, содержащая произвольную комбинацию 0 и 1, разделенных пробелом. Записать в файл, задаваемый вторым аргументом командной строки, два числа - количество последовательностей из 1 и 0. Примечание: unique(), count().</t>
-  </si>
-  <si>
-    <t>input.txt                                  output.txt
-1 0 1 1                                               2 1
-0 0 0                                                  0 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">input.txt                                  output.txt
-2                                                          2
-13     
-4                                                        104
-3 1 8 100                                                    </t>
-  </si>
-  <si>
-    <t>Исключить из массива первый четный элемент, следующий за максимальным. На вход подается число N - количество элеменетов массива, элементы массива. На выход - позиция элемента, его значение, массив после удаления элемента. Примечание: resize(), copy() и ofstream_iterator (для вывода вектора), max_element(), find_if с лямбда-функцией для определение четности число ([](тип значение) {код}), distance(), erase().</t>
-  </si>
-  <si>
-    <t>Даны 12 csv-файлов с логинами и их зашифрованными через радуждные таблицы версиями. Пользователь вводит зашифрованный логин, необходимо найти в фалах его оригинал.</t>
+Если условия не выполнены, вывести, по какому индексу в строке произошла ошибка.
+Реализовать с помощью std::stack.
+Напишите функцию balance, которая проверяет выполнение баланса скобок. 
+Функция принимает строку, возращает std::pair&lt;int, int&gt;. 
+Если баланс выполняется,  на первое место записывается 1, на второе -1. 
+Если не выполняется, на первое записывается 0, на второе - индекс, где произошла ошибка.
+Примечание: в строке могут быть другие символы.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C++, сложность D, семестр 3, STL, stack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В функцию numberOfSequences подаются две строки - названия входного и выходного файла.
+В единственной строке входного файла находится последовательность, 
+содержащая произвольную комбинацию 0 и 1, разделенных пробелом.
+Записать во второй файл (выходной) два числа - количество последовательностей из 1 и 0. 
+Примечание: использовать unique(), count().
+Примечание 2: данные в выходном файле перезаписываются. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C++, сложность D, семестр 3, STL, работа с файлами</t>
+  </si>
+  <si>
+    <t>В функцию playingCards подаются две строки - названия входного и выходного файла.
+Первая строка входного файла содержит одно четное натуральное число N. 
+Вторая строка входного файла содержит ровно N чисел - числа, написанные на игральных карточках. 
+Все числа в строке разделяются одиночными пробелами. Игроки выбирают закрытые карточки, 
+первый выбирает половину карточек, второй забирает оставшуюся половину. 
+Во второй файл записать максимальный выигрыш, который можно получить, т.е разница между суммами чисел на карточках. 
+Примечание: используйте sort()/partial_sort(), reverve(), accumulate(), std::greater</t>
+  </si>
+  <si>
+    <t>C++, сложность D, семестр 3, STL, работа с файлами</t>
+  </si>
+  <si>
+    <t>Напишите функцию deleteElement, которая исключит из вектора первый четный элемент, следующий за максимальным. 
+На вход подается вектор целых чисел. 
+На выход - напечатать позицию элемента и его значение, вернуть массив после удаления элемента. 
+Примечание: resize(), copy() и ofstream_iterator (для вывода вектора), max_element(), 
+find_if с лямбда-функцией для определение четности число ([](тип значение) {код}), distance(), erase().</t>
+  </si>
+  <si>
+    <t>C++, сложность D, семестр 3, STL, вектор</t>
+  </si>
+  <si>
+    <t>C++, сложность E, семестр 3</t>
+  </si>
+  <si>
+    <t>input: 10011_2 171_8
+output: 10001100</t>
+  </si>
+  <si>
+    <t>Даны 12 csv-файлов с логинами и их зашифрованными через радуждные таблицы версиями. 
+Пользователь вводит зашифрованный логин, необходимо найти в файлах его оригинал.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Разработать шаблонный класс Pair, хранящий пару значений разных типов. Класс должен:
+● реализовывать методы для доступа к значениям и задания значений;
+● реализовывать операторы сравнения (==, !=);
+● реализовывать оператор сложения, складывающий соответствующие элементы пары;
+● реализовывать оператор выставки в поток (&lt;&lt;), выводящий в консоль пару в виде “(first, second)”; 
+● реализовать оператор извлечения из потока (&gt;&gt;), принимающий два значения из консоли и заполняющий ими пару строк;
+● метод, принимающий два значения и возвращающий составленную из них пару;
+● метод, принимающий пару и возвращающий пару, в которой первое значение поставлено
+  на место второго, второе – на место первого </t>
+  </si>
+  <si>
+    <t>C++, сложность C, семестр 3, ООП</t>
+  </si>
+  <si>
+    <t>Написать программу, которая построчно объединяет файлы, переданные ей как аргументы командной строки, 
+и выводит их в новый текстовый файл.
+Передачу имен файлов реализовать через аргументы командной строки.
+Объединение происходит таким образом, что сначала выводятся первые строки всех файлов по 
+порядку следования, потом вторые, третьи и т. д.
+Если какие-то из файлов не могут быть найдены или открыты, программа должна выдать 
+предупреждение об этом в стандартный вывод ошибок (cerr) и продолжить работу, игнорируя неоткрытые файлы.
+Example:</t>
+  </si>
+  <si>
+    <t>input:
+Файл 1.txt:
+aa
+bb
+cc
+Файл 2.txt:
+0
+1
+Файл 3.txt:
+hey
+output:
+aa
+0
+hey
+bb
+1
+cc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C++, сложность D, семестр 3, работа с файлами</t>
+  </si>
+  <si>
+    <t>Дано N чисел, требуется выяснить, сколько среди них различных.
+В первой строке дано число N – количество чисел. (1 &lt;= N &lt;= 100000) 
+Во второй строке даны через пробел N чисел, каждое не превышает 2*10^9 по модулю.
+Выведите число, равное количеству различных чисел среди данных.
+Примечание: использовать STL.</t>
+  </si>
+  <si>
+    <t>input:
+5
+1 0 1 2 0
+output:
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C++, сложность D, семестр 3, STL</t>
+  </si>
+  <si>
+    <t>Напишите программу, которая моделирует игру в пьяницу и определяет, кто выигрывает. 
+В игре участвует 10 карт, имеющих значения от 0 до 9, большая карта побеждает меньшую, карта со значением 0 побеждает карту 9.
+Программа получает на вход две строки: первая строка содержит 5 чисел, разделенных пробелами — номера карт первого игрока, 
+вторая – аналогично 5 карт второго игрока. Карты перечислены сверху вниз, то есть каждая строка начинается с той карты, которая будет открыта первой.
+Программа должна определить, кто выигрывает при данной раздаче, и вывести слово first или second, после чего вывести количество ходов, 
+сделанных до выигрыша. Если на протяжении 10^6 ходов игра не заканчивается, программа должна вывести слово botva.
+Примечание: использовать STL.</t>
+  </si>
+  <si>
+    <t>input:
+1 3 5 7 9
+2 4 6 8 0
+output:
+second 5</t>
+  </si>
+  <si>
+    <t>На складе хранятся контейнеры с товарами N различных видов. Все контейнеры составлены в N стопок. 
+В каждой стопке могут находиться контейнеры с товарами любых видов (стопка может быть изначально пустой).
+Автопогрузчик может взять верхний контейнер из любой стопки и поставить его сверху в любую стопку. 
+Необходимо расставить все контейнеры с товаром первого вида в первую стопку, второго вида – во вторую стопку и т.д.
+Программа должна вывести последовательность действий автопогрузчика или сообщение о том, что задача решения не имеет.
+В первой строке входных данных записано одно натуральное число N, не превосходящее 500. 
+В следующих N строках описаны стопки контейнеров: сначала записано число ki – количество контейнеров в стопке, 
+а затем ki чисел – виды товара в контейнерах в данной стопке, снизу вверх. В каждой стопке вначале 
+не более 500 контейнеров (в процессе переноса контейнеров это ограничение может быть нарушено).
+Программа должна вывести описание действий автопогрузчика: для каждого действия напечатать два 
+числа – из какой стопки брать контейнер и в какую стопку класть. (Обратите внимание, что минимизировать 
+количество операций автопогрузчика не требуется.) Если задача не имеет решения, необходимо вывести одно число 0. 
+Если контейнеры изначально правильно размещены по стопкам, то  выводить ничего не нужно.
+римечание: использовать STL.</t>
+  </si>
+  <si>
+    <t>input:
+3
+4 1 2 3 2
+0
+0
+output:
+1 2
+1 3
+1 2
+Объяснение примера. Изначально в первой стопке лежат четыре контейнера – снизу контейнер с товаром первого вида, 
+над ним – с товаром второго вида, над ним третьего, и сверху еще один контейнер с товаром второго вида. Вторая и третья стопки – пусты.</t>
+  </si>
+  <si>
+    <t>C++, сложность C, семестр 3, STL, stack</t>
+  </si>
+  <si>
+    <t>Для транспортирования материалов из цеха А в цех В используется конвейер. Материалы упаковываются в одинаковые контейнеры и размещаются на
+ленте один за одним в порядке изготовления в цехе А. Каждый контейнер имеет степень срочности обработки в цехе В. Для упорядочивания 
+контейнеров по степени срочности используют накопитель, который находится в конце конвейера перед входом в цех В. Накопитель работает пошагово, 
+на каждом шаге возможны следующие действия:
+* накопитель перемещает первый контейнер из ленты в цех В;
+* накопитель перемещает первый контейнер из строки в склад (в складе каждый следующий контейнер помещается на предыдущий);
+* накопитель перемещает верхний контейнер из склада в цех В.
+Напишите программу, которая по последовательности контейнеров определит, можно ли упорядочить их по степени срочности пользуясь описанным накопителем.
+Входной файл в первой строке содержит количество тестов N. Далее следует N строк, каждый из которых описывает отдельный тест и содержит целое 
+число K (1 ≤ K ≤ 10000) — количество контейнеров в последовательности и K действительных чисел — степеней срочности контейнеров в порядке 
+их поступления из цеха А (меньшим числам соответствует большая степень срочности).
+Выходные данные
+Каждая строка выходного файла должна содержать ответ для одного теста. Необходимо вывести 1, если необходимое упорядочивание возможно, или 0 в противном случае.</t>
+  </si>
+  <si>
+    <t>input:
+2
+2 2.9 2.1
+3 5.6 9.0 2.0
+output:
+1</t>
+  </si>
+  <si>
+    <t>На барже располагается K грузовых отсеков. В каждый отсек можно поместить некоторое количество бочек с одним из 10 000 видов топлива.
+Причём извлечь бочку из отсека можно лишь в случае, если все бочки, помещённые в этот отсек после неё, уже были извлечены.
+Таким образом в каждый момент времени в каждом непустом отсеке имеется ровно одна бочка, которую можно извлечь не трогая остальных. 
+Будем называть такие бочки крайними.
+Изначально баржа пуста. Затем она последовательно проплывает через N доков, причём в каждом доке на баржу либо погружается бочка
+с некоторым видом топлива в некоторый отсек, либо выгружается крайняя бочка из некоторого отсека. Однако, если указанный отсек пуст,
+либо если выгруженная бочка содержит не тот вид топлива, который ожидалось, следует зафиксировать ошибку. Если на баржу оказывается
+погружено более P бочек или если после прохождения всех доков она не стала пуста, следует также зафиксировать ошибку.
+От вас требуется либо указать максимальное количество бочек, которые одновременно пребывали на барже либо зафиксировать ошибку.
+В первой строке три целых числа N, K и P (1 ≤ N, K, P ≤ 100 000). Далее следует N строк с описанием действия, выполняемого в очередном доке. Если в нём происходит погрузка, то строка имеет вид «+ A B», где A — номер отсека, в который помещается бочка, а B — номер вида топлива в ней. Если же док занимается разгрузкой, то строка имеет вид «- A B», где A — номер отсека, из которого извлекается бочка, а B — номер ожидаемого вида топлива.
+Вывести либо одно число, равное искомому максимуму в случае безошибочного прохождения баржой маршрута, либо вывести слово «Error» в противном случае.</t>
+  </si>
+  <si>
+    <t>input:
+6 1 2
++ 1 1
++ 1 2
+- 1 2
+- 1 1
++ 1 3
+- 1 3
+output:
+2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C++, сложность C, семестр 3, STL</t>
+  </si>
+  <si>
+    <t>На секретную базу в Арктике поступила шифровка – последовательность из n десятичных цифр. Она содержит номер секретной базы в Антарктиде, 
+который является последовательностью из k десятичных цифр. При этом для того, чтобы отличить его от ненужной Вам информации, он повторен 
+в шифровке хотя бы два раза (возможно, эти два вхождения перекрываются).
+Напишите программу, которая по шифровке и длине номера секретной базы определяет, содержит ли шифровка номер базы. Учтите, что у базы может
+быть несколько номеров, и все они могут быть переданы в шифровке.
+Первая строка входного файла INPUT.TXT содержит два целых числа: n (1 ≤ n ≤ 10^5) и k (1 ≤ k ≤ 5) – длину шифровки и длину номера секретной 
+базы соответственно. Вторая строка содержит n цифр – шифровку. Помните, что цифры в шифровке не разделяются пробелами.
+В выходной файл OUTPUT.TXT выведите «YES», если шифровка содержит номер секретной базы, и «NO» в противном случае.</t>
+  </si>
+  <si>
+    <t>input: 
+10 5
+0123456789
+output:
+NO
+input:
+13 2
+0123400056789
+output:
+YES</t>
+  </si>
+  <si>
+    <t>C++, сложность C, семестр 3, работа с файлами</t>
+  </si>
+  <si>
+    <t>В первой строке входного файла INPUT.TXT находится два числа N и M (1 ≤ N ≤ 103, 1 ≤ M ≤ 105). В следующих N строках находится по одному
+слову из словаря. Все слова состоят из строчных английских букв. Длина каждого слова не превышает 20. Каждое слово состоит хотя бы из 
+одного символа. Лишних пробелов перед словом и после него нет.
+В следующих M строках находится текст сочинения. Текст состоит из заглавных и строчных английских букв, пробелов и знаков препинания: 
+точек (.), запятых (,), двоеточий (:), точек с запятыми (;), тире (-), апострофов ('), кавычек ("), восклицательных (!) и вопросительных (?) знаков.
+Общая длина текста не превосходит 104 символов. В данной задаче большие и маленькие буквы в словах не различаются.
+В выходной файл OUTPUT.TXT выведите «Everything is going to be OK.», если с сочинением все в порядке. Если не все слова из текста встречаются в 
+словаре, выведите «Some words from the text are unknown.». Если же предыдущее неверно, но некоторые слова из словаря не встречаются в тексте, 
+выведите «The usage of the vocabulary is not perfect.».</t>
+  </si>
+  <si>
+    <t>C++, сложность D, семестр 3, работа с файлами</t>
+  </si>
+  <si>
+    <t>№ INPUT.TXT             OUTPUT.TXT
+1 3 1
+    am
+    bill
+    i
+    I am Bill, am I?     Everything is going to be OK.
+2 2 2
+    seven
+    day
+    On the
+    seventh day             Some words from the text are unknown.
+3 4 1
+    vocabulary
+    wide
+    too
+    much
+    Too wide vocabulary. The usage of the vocabulary is not perfect.</t>
+  </si>
+  <si>
+    <t>Напишите функцию sumNumber, которая принимает две строки - числа в разных системах счисления (со 2 по 36)
+и выводит их сумму в двоичной системе счисления. Числа представлены в виде: число_системаСчисления</t>
+  </si>
+  <si>
+    <t>input: 
+(){}([])
+output:
+1 -1
+:
+input: 
+([{aaa})]
+output:
+0 7</t>
+  </si>
+  <si>
+    <t>input: 
+1 0 1 1
+output:
+2 1
+input: 
+0 0 0 
+output:
+0 1</t>
+  </si>
+  <si>
+    <t>input: 
+2
+1 3
+output:
+2
+input: 
+4
+3 1 8 100  
+output:
+104</t>
   </si>
 </sst>
 </file>
@@ -152,19 +432,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -452,21 +726,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B21" sqref="B20:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.26953125" customWidth="1"/>
-    <col min="2" max="2" width="64.81640625" customWidth="1"/>
-    <col min="3" max="3" width="47.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.453125" customWidth="1"/>
+    <col min="1" max="1" width="64.85546875" customWidth="1"/>
+    <col min="2" max="2" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,133 +749,165 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="5" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" ht="157.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="5" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" ht="117.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+    </row>
+    <row r="14" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="300" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="330" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>